<commit_message>
update nav interne review
</commit_message>
<xml_diff>
--- a/0. imkl 3.0 release candidate-intern/imkl3.0.0rc-intern-review.xlsx
+++ b/0. imkl 3.0 release candidate-intern/imkl3.0.0rc-intern-review.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\p.janssen.GNM\Documents\Github\imkl-werkomgeving\0. imkl 3.0 release candidate-intern\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08EA58BB-642C-4283-BDB9-044CFF2A5DF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB76BFF4-3FD2-4CFF-92B8-B9D365AFB7A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{42CEC8C0-599F-4045-81A0-1EFE4C6D1A60}"/>
+    <workbookView xWindow="-96" yWindow="1740" windowWidth="22356" windowHeight="10596" xr2:uid="{42CEC8C0-599F-4045-81A0-1EFE4C6D1A60}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -120,7 +120,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="109">
   <si>
     <t>nummer</t>
   </si>
@@ -466,7 +466,30 @@
     <t>verwerkt in uml</t>
   </si>
   <si>
-    <t>verwerkt in uml en daarmee ook in standaard document</t>
+    <t>verwerkt in uml en daarmee ook in modeldocument (na generatie objectcat)</t>
+  </si>
+  <si>
+    <t>verwerkt in uml
+verwerkt in xsd
+verwerkt in changelog</t>
+  </si>
+  <si>
+    <t>is verwerkt in waardelijst excel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">changlog item 39 is verwijderd.
+Verwerkt in UML: Constraints zijn aangepast/herformuleerd op basis van voorstel.
+Verwerkt in changelog: herformulering van constraints op GebiedsinformatieAanvraag
+</t>
+  </si>
+  <si>
+    <t>is verwerkt in UML diagrammen en verwijderd uit model.</t>
+  </si>
+  <si>
+    <t>is verwerkt in extraRegels excel</t>
+  </si>
+  <si>
+    <t>verwerkt. Dit changelog item is nu item 42 geworden</t>
   </si>
 </sst>
 </file>
@@ -1105,8 +1128,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19C97A4D-2E1A-458B-A8A3-14C33881EDAE}">
   <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1358,7 +1381,9 @@
       <c r="F12" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="G12" s="23"/>
+      <c r="G12" s="23" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="13" spans="1:7" ht="57.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="5">
@@ -1379,7 +1404,9 @@
       <c r="F13" s="22" t="s">
         <v>94</v>
       </c>
-      <c r="G13" s="23"/>
+      <c r="G13" s="23" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="14" spans="1:7" ht="55.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="5">
@@ -1400,7 +1427,9 @@
       <c r="F14" s="22" t="s">
         <v>94</v>
       </c>
-      <c r="G14" s="23"/>
+      <c r="G14" s="23" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="15" spans="1:7" ht="174.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="5">
@@ -1421,6 +1450,9 @@
       <c r="F15" s="5" t="s">
         <v>81</v>
       </c>
+      <c r="G15" s="14" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="16" spans="1:7" ht="21" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="5">
@@ -1459,6 +1491,9 @@
       <c r="F17" s="22" t="s">
         <v>95</v>
       </c>
+      <c r="G17" s="4" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="18" spans="1:7" ht="75.599999999999994" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="5">
@@ -1479,7 +1514,9 @@
       <c r="F18" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="G18" s="7"/>
+      <c r="G18" s="7" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="19" spans="1:7" ht="21" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="5">
@@ -1500,7 +1537,9 @@
       <c r="F19" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="G19" s="7"/>
+      <c r="G19" s="7" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="20" spans="1:7" ht="40.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="5">
@@ -1520,6 +1559,9 @@
       </c>
       <c r="F20" s="5" t="s">
         <v>80</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="80.400000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
update naar versie 3.0 extern
</commit_message>
<xml_diff>
--- a/0. imkl 3.0 release candidate-intern/imkl3.0.0rc-intern-review.xlsx
+++ b/0. imkl 3.0 release candidate-intern/imkl3.0.0rc-intern-review.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\p.janssen.GNM\Documents\Github\imkl-werkomgeving\0. imkl 3.0 release candidate-intern\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70ADC2D6-A698-4726-9C3F-2CC95401BE5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00DF80AA-FDF6-4F0F-BF27-C980BBB4DF12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-8010" windowWidth="29040" windowHeight="15720" xr2:uid="{42CEC8C0-599F-4045-81A0-1EFE4C6D1A60}"/>
   </bookViews>
@@ -120,7 +120,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="124">
   <si>
     <t>nummer</t>
   </si>
@@ -404,9 +404,6 @@
     <t>akkoord. Bij changelog item 39 staat inderdaad een fout. Calamiteitmelding moet weg. Constraint in 'Gebiedsinformatieaanvraag' is niet correct</t>
   </si>
   <si>
-    <t>akkoord. Wordt uitgezocht.</t>
-  </si>
-  <si>
     <t>Akkoord. Wordt aangepast. fysiekeIdentificatie
 Definitie: Merkband, nummer of print op de buis.
 Toelichting: Maximaal 64 karakters.</t>
@@ -428,9 +425,6 @@
   </si>
   <si>
     <t>Akkoord: Wordt aangepast</t>
-  </si>
-  <si>
-    <t>Akkoord. Deze wordt op 0..1 gezet en met een regel voor kabelbed verplicht.</t>
   </si>
   <si>
     <t>Wordt als 'infiltratievoorziening' opgenomen. Zie issue 291</t>
@@ -509,6 +503,54 @@
   </si>
   <si>
     <t>wordt als voorstel uitgewerkt</t>
+  </si>
+  <si>
+    <t>akkoord. Wordt uitgezocht. Ook de het attribuut ligging moet optioneel worden
+Het is niet de bedoeling dat er er verplicht een bestand meegeleverd wordt</t>
+  </si>
+  <si>
+    <t>verwerkt.
+Beide attributen zijn optioneel gemaakt.
+Verwerkt in UML.
+Verwerkt in XSD.
+Verwerkt in changelog.</t>
+  </si>
+  <si>
+    <t>is verwerkt in UML</t>
+  </si>
+  <si>
+    <t>geen aanpassing nodig</t>
+  </si>
+  <si>
+    <t>is verwerkt in UML
+is verwerkt in changelog
+is verwerkt in XSD</t>
+  </si>
+  <si>
+    <t>is verwerkt in uml</t>
+  </si>
+  <si>
+    <t>is verwerkt in doc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">is verwerkt in waardelijst excel
+is verwerkt in uml
+is verwerkt in XSD
+</t>
+  </si>
+  <si>
+    <t>is verwerkt in waardelijst excel
+is verwerkt in uml
+is verwerkt in XSD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">verwerkt in uml
+verwerkt in IMKL-extraRegels
+verwerkt in XSD
+</t>
+  </si>
+  <si>
+    <t>Akkoord. Deze wordt op 0..1 gezet en met een regel voor kabelbed en duct verplicht.</t>
   </si>
 </sst>
 </file>
@@ -1139,7 +1181,7 @@
   <dimension ref="A1:G41"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F36" sqref="F36"/>
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1164,7 +1206,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="16" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E1" s="19" t="s">
         <v>2</v>
@@ -1173,7 +1215,7 @@
         <v>22</v>
       </c>
       <c r="G1" s="23" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="51.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1196,7 +1238,7 @@
         <v>72</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="49.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1219,7 +1261,7 @@
         <v>73</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="49.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1238,7 +1280,7 @@
         <v>74</v>
       </c>
       <c r="G4" s="23" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="49.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1257,7 +1299,7 @@
         <v>75</v>
       </c>
       <c r="G5" s="23" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="49.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1314,7 +1356,7 @@
         <v>78</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="106.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1337,7 +1379,7 @@
         <v>79</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="32.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1358,7 +1400,7 @@
         <v>80</v>
       </c>
       <c r="G10" s="23" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="61.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1381,7 +1423,7 @@
         <v>80</v>
       </c>
       <c r="G11" s="24" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="94.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1399,10 +1441,10 @@
         <v>29</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="57.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1422,10 +1464,10 @@
         <v>31</v>
       </c>
       <c r="F13" s="21" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>104</v>
+        <v>120</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="55.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1445,10 +1487,10 @@
         <v>31</v>
       </c>
       <c r="F14" s="21" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>104</v>
+        <v>121</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="174.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1471,7 +1513,7 @@
         <v>81</v>
       </c>
       <c r="G15" s="24" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="21" thickBot="1" x14ac:dyDescent="0.35">
@@ -1510,10 +1552,10 @@
         <v>37</v>
       </c>
       <c r="F17" s="21" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G17" s="23" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="75.599999999999994" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1536,7 +1578,7 @@
         <v>80</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="21" thickBot="1" x14ac:dyDescent="0.35">
@@ -1559,7 +1601,7 @@
         <v>80</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="40.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1581,8 +1623,8 @@
       <c r="F20" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="G20" s="23" t="s">
-        <v>108</v>
+      <c r="G20" s="24" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="80.400000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1603,9 +1645,11 @@
         <v>45</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="G21" s="23"/>
+        <v>113</v>
+      </c>
+      <c r="G21" s="24" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="22" spans="1:7" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="5">
@@ -1641,9 +1685,11 @@
         <v>52</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="G23" s="23"/>
+        <v>82</v>
+      </c>
+      <c r="G23" s="23" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="24" spans="1:7" ht="96" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="5">
@@ -1663,9 +1709,11 @@
         <v>53</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="G24" s="23"/>
+        <v>83</v>
+      </c>
+      <c r="G24" s="23" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="25" spans="1:7" ht="105" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="5">
@@ -1685,9 +1733,11 @@
         <v>54</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="G25" s="23"/>
+        <v>84</v>
+      </c>
+      <c r="G25" s="23" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="26" spans="1:7" ht="61.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="5">
@@ -1707,9 +1757,11 @@
         <v>55</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="G26" s="23"/>
+        <v>85</v>
+      </c>
+      <c r="G26" s="24" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="27" spans="1:7" ht="120" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="5">
@@ -1727,9 +1779,11 @@
         <v>56</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="G27" s="23"/>
+        <v>86</v>
+      </c>
+      <c r="G27" s="23" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="28" spans="1:7" ht="142.80000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="5">
@@ -1747,9 +1801,11 @@
         <v>57</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="G28" s="23"/>
+        <v>87</v>
+      </c>
+      <c r="G28" s="23" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="29" spans="1:7" ht="33.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="5">
@@ -1783,9 +1839,11 @@
         <v>59</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="G30" s="23"/>
+        <v>88</v>
+      </c>
+      <c r="G30" s="23" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="31" spans="1:7" ht="90" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="5">
@@ -1803,9 +1861,11 @@
         <v>60</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="G31" s="23"/>
+        <v>88</v>
+      </c>
+      <c r="G31" s="23" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="32" spans="1:7" ht="39.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="5">
@@ -1823,11 +1883,13 @@
         <v>61</v>
       </c>
       <c r="F32" s="21" t="s">
-        <v>96</v>
-      </c>
-      <c r="G32" s="23"/>
-    </row>
-    <row r="33" spans="1:7" ht="41.4" thickBot="1" x14ac:dyDescent="0.35">
+        <v>94</v>
+      </c>
+      <c r="G32" s="23" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="5">
         <f>+A32+1</f>
         <v>28</v>
@@ -1843,9 +1905,11 @@
         <v>62</v>
       </c>
       <c r="F33" s="21" t="s">
-        <v>97</v>
-      </c>
-      <c r="G33" s="23"/>
+        <v>95</v>
+      </c>
+      <c r="G33" s="24" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="34" spans="1:7" ht="41.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="5">
@@ -1863,9 +1927,11 @@
         <v>63</v>
       </c>
       <c r="F34" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="G34" s="23"/>
+        <v>89</v>
+      </c>
+      <c r="G34" s="23" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="35" spans="1:7" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="5">
@@ -1885,9 +1951,11 @@
         <v>67</v>
       </c>
       <c r="F35" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="G35" s="23"/>
+        <v>123</v>
+      </c>
+      <c r="G35" s="24" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="36" spans="1:7" ht="72" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="5">
@@ -1901,10 +1969,10 @@
       </c>
       <c r="D36" s="5"/>
       <c r="E36" s="6" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F36" s="6" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G36" s="23"/>
     </row>

</xml_diff>

<commit_message>
klaar maken voor pub
</commit_message>
<xml_diff>
--- a/0. imkl 3.0 release candidate-intern/imkl3.0.0rc-intern-review.xlsx
+++ b/0. imkl 3.0 release candidate-intern/imkl3.0.0rc-intern-review.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\p.janssen.GNM\Documents\Github\imkl-werkomgeving\0. imkl 3.0 release candidate-intern\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{843B7B23-4664-4BED-ADCD-13822E3249D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D42AFAED-004D-4F00-82EB-584F3AA0C49E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26880" yWindow="-5970" windowWidth="21600" windowHeight="11235" activeTab="1" xr2:uid="{42CEC8C0-599F-4045-81A0-1EFE4C6D1A60}"/>
+    <workbookView xWindow="28680" yWindow="-5445" windowWidth="38640" windowHeight="21120" xr2:uid="{42CEC8C0-599F-4045-81A0-1EFE4C6D1A60}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -120,7 +120,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="125">
   <si>
     <t>nummer</t>
   </si>
@@ -551,6 +551,9 @@
   </si>
   <si>
     <t>Akkoord. Deze wordt op 0..1 gezet en met een regel voor kabelbed en duct verplicht.</t>
+  </si>
+  <si>
+    <t>niet verwerkt, blijft een externe contole</t>
   </si>
 </sst>
 </file>
@@ -599,7 +602,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -621,6 +624,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -677,7 +686,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -703,9 +712,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -748,6 +754,21 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1180,8 +1201,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19C97A4D-2E1A-458B-A8A3-14C33881EDAE}">
   <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1189,32 +1210,32 @@
     <col min="1" max="1" width="4" customWidth="1"/>
     <col min="2" max="2" width="12.77734375" customWidth="1"/>
     <col min="3" max="3" width="21.5546875" customWidth="1"/>
-    <col min="4" max="4" width="38.33203125" style="13" customWidth="1"/>
-    <col min="5" max="5" width="52.44140625" style="14" customWidth="1"/>
+    <col min="4" max="4" width="38.33203125" style="12" customWidth="1"/>
+    <col min="5" max="5" width="52.44140625" style="13" customWidth="1"/>
     <col min="6" max="6" width="27" customWidth="1"/>
     <col min="7" max="7" width="40.33203125" style="4" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="D1" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="E1" s="19" t="s">
+      <c r="E1" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="20" t="s">
+      <c r="F1" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="G1" s="23" t="s">
+      <c r="G1" s="22" t="s">
         <v>96</v>
       </c>
     </row>
@@ -1279,7 +1300,7 @@
       <c r="F4" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="G4" s="23" t="s">
+      <c r="G4" s="22" t="s">
         <v>97</v>
       </c>
     </row>
@@ -1298,7 +1319,7 @@
       <c r="F5" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="G5" s="23" t="s">
+      <c r="G5" s="22" t="s">
         <v>98</v>
       </c>
     </row>
@@ -1317,7 +1338,7 @@
       <c r="F6" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="G6" s="23" t="s">
+      <c r="G6" s="22" t="s">
         <v>110</v>
       </c>
     </row>
@@ -1333,31 +1354,33 @@
       <c r="E7" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="F7" s="22" t="s">
+      <c r="F7" s="21" t="s">
         <v>77</v>
       </c>
-      <c r="G7" s="23"/>
+      <c r="G7" s="22" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="8" spans="1:7" ht="51.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="5">
+      <c r="A8" s="24">
         <v>3</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="E8" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="F8" s="5" t="s">
+      <c r="F8" s="24" t="s">
         <v>78</v>
       </c>
-      <c r="G8" s="5" t="s">
+      <c r="G8" s="24" t="s">
         <v>109</v>
       </c>
     </row>
@@ -1401,7 +1424,7 @@
       <c r="F10" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="G10" s="23" t="s">
+      <c r="G10" s="22" t="s">
         <v>99</v>
       </c>
     </row>
@@ -1424,51 +1447,51 @@
       <c r="F11" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="G11" s="24" t="s">
+      <c r="G11" s="23" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="94.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="5">
+      <c r="A12" s="24">
         <v>7</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5" t="s">
+      <c r="C12" s="24"/>
+      <c r="D12" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="E12" s="6" t="s">
+      <c r="E12" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="F12" s="5" t="s">
+      <c r="F12" s="24" t="s">
         <v>90</v>
       </c>
-      <c r="G12" s="5" t="s">
+      <c r="G12" s="24" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="57.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="5">
+      <c r="A13" s="24">
         <v>8</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D13" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="E13" s="6" t="s">
+      <c r="E13" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="F13" s="21" t="s">
+      <c r="F13" s="24" t="s">
         <v>92</v>
       </c>
-      <c r="G13" s="5" t="s">
+      <c r="G13" s="24" t="s">
         <v>120</v>
       </c>
     </row>
@@ -1488,7 +1511,7 @@
       <c r="E14" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="F14" s="21" t="s">
+      <c r="F14" s="20" t="s">
         <v>92</v>
       </c>
       <c r="G14" s="5" t="s">
@@ -1514,7 +1537,7 @@
       <c r="F15" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="G15" s="24" t="s">
+      <c r="G15" s="23" t="s">
         <v>103</v>
       </c>
     </row>
@@ -1535,28 +1558,28 @@
         <v>35</v>
       </c>
       <c r="F16" s="5"/>
-      <c r="G16" s="23"/>
+      <c r="G16" s="22"/>
     </row>
     <row r="17" spans="1:7" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="5">
+      <c r="A17" s="24">
         <v>12</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="C17" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="D17" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="E17" s="6" t="s">
+      <c r="E17" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="F17" s="21" t="s">
+      <c r="F17" s="24" t="s">
         <v>93</v>
       </c>
-      <c r="G17" s="23" t="s">
+      <c r="G17" s="26" t="s">
         <v>102</v>
       </c>
     </row>
@@ -1625,7 +1648,7 @@
       <c r="F20" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="G20" s="24" t="s">
+      <c r="G20" s="23" t="s">
         <v>106</v>
       </c>
     </row>
@@ -1649,7 +1672,7 @@
       <c r="F21" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="G21" s="24" t="s">
+      <c r="G21" s="23" t="s">
         <v>114</v>
       </c>
     </row>
@@ -1667,7 +1690,7 @@
       </c>
       <c r="E22" s="6"/>
       <c r="F22" s="5"/>
-      <c r="G22" s="23"/>
+      <c r="G22" s="22"/>
     </row>
     <row r="23" spans="1:7" ht="106.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="5">
@@ -1689,7 +1712,7 @@
       <c r="F23" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="G23" s="23" t="s">
+      <c r="G23" s="22" t="s">
         <v>115</v>
       </c>
     </row>
@@ -1713,7 +1736,7 @@
       <c r="F24" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="G24" s="23" t="s">
+      <c r="G24" s="22" t="s">
         <v>116</v>
       </c>
     </row>
@@ -1737,31 +1760,31 @@
       <c r="F25" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="G25" s="23" t="s">
+      <c r="G25" s="22" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="61.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="5">
+      <c r="A26" s="24">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="B26" s="5" t="s">
+      <c r="B26" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="C26" s="5" t="s">
+      <c r="C26" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="D26" s="5" t="s">
+      <c r="D26" s="24" t="s">
         <v>64</v>
       </c>
-      <c r="E26" s="6" t="s">
+      <c r="E26" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="F26" s="5" t="s">
+      <c r="F26" s="24" t="s">
         <v>85</v>
       </c>
-      <c r="G26" s="24" t="s">
+      <c r="G26" s="27" t="s">
         <v>117</v>
       </c>
     </row>
@@ -1783,7 +1806,7 @@
       <c r="F27" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="G27" s="23" t="s">
+      <c r="G27" s="22" t="s">
         <v>118</v>
       </c>
     </row>
@@ -1805,7 +1828,7 @@
       <c r="F28" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="G28" s="23" t="s">
+      <c r="G28" s="22" t="s">
         <v>116</v>
       </c>
     </row>
@@ -1823,7 +1846,7 @@
       </c>
       <c r="E29" s="6"/>
       <c r="F29" s="5"/>
-      <c r="G29" s="23"/>
+      <c r="G29" s="22"/>
     </row>
     <row r="30" spans="1:7" ht="85.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="5">
@@ -1843,7 +1866,7 @@
       <c r="F30" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="G30" s="23" t="s">
+      <c r="G30" s="22" t="s">
         <v>119</v>
       </c>
     </row>
@@ -1865,51 +1888,51 @@
       <c r="F31" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="G31" s="23" t="s">
+      <c r="G31" s="22" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="39.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="5">
+      <c r="A32" s="24">
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
-      <c r="B32" s="5" t="s">
+      <c r="B32" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="C32" s="5" t="s">
+      <c r="C32" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="D32" s="5"/>
-      <c r="E32" s="6" t="s">
+      <c r="D32" s="24"/>
+      <c r="E32" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="F32" s="21" t="s">
+      <c r="F32" s="24" t="s">
         <v>94</v>
       </c>
-      <c r="G32" s="23" t="s">
+      <c r="G32" s="26" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="5">
+      <c r="A33" s="24">
         <f>+A32+1</f>
         <v>28</v>
       </c>
-      <c r="B33" s="5" t="s">
+      <c r="B33" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="C33" s="5" t="s">
+      <c r="C33" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="D33" s="5"/>
-      <c r="E33" s="6" t="s">
+      <c r="D33" s="24"/>
+      <c r="E33" s="25" t="s">
         <v>62</v>
       </c>
-      <c r="F33" s="21" t="s">
+      <c r="F33" s="24" t="s">
         <v>95</v>
       </c>
-      <c r="G33" s="24" t="s">
+      <c r="G33" s="27" t="s">
         <v>121</v>
       </c>
     </row>
@@ -1931,31 +1954,31 @@
       <c r="F34" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="G34" s="23" t="s">
+      <c r="G34" s="22" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="5">
+      <c r="A35" s="24">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="B35" s="5" t="s">
+      <c r="B35" s="24" t="s">
         <v>65</v>
       </c>
-      <c r="C35" s="5" t="s">
+      <c r="C35" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="D35" s="5" t="s">
+      <c r="D35" s="24" t="s">
         <v>66</v>
       </c>
-      <c r="E35" s="9" t="s">
+      <c r="E35" s="28" t="s">
         <v>67</v>
       </c>
-      <c r="F35" s="6" t="s">
+      <c r="F35" s="25" t="s">
         <v>123</v>
       </c>
-      <c r="G35" s="24" t="s">
+      <c r="G35" s="27" t="s">
         <v>122</v>
       </c>
     </row>
@@ -1976,7 +1999,7 @@
       <c r="F36" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="G36" s="23"/>
+      <c r="G36" s="22"/>
     </row>
     <row r="37" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="5"/>
@@ -1984,8 +2007,8 @@
       <c r="C37" s="5"/>
       <c r="D37" s="5"/>
       <c r="E37" s="6"/>
-      <c r="F37" s="10"/>
-      <c r="G37" s="23"/>
+      <c r="F37" s="9"/>
+      <c r="G37" s="22"/>
     </row>
     <row r="38" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="5"/>
@@ -1994,7 +2017,7 @@
       <c r="D38" s="5"/>
       <c r="E38" s="6"/>
       <c r="F38" s="5"/>
-      <c r="G38" s="23"/>
+      <c r="G38" s="22"/>
     </row>
     <row r="39" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="5"/>
@@ -2003,7 +2026,7 @@
       <c r="D39" s="5"/>
       <c r="E39" s="6"/>
       <c r="F39" s="5"/>
-      <c r="G39" s="23"/>
+      <c r="G39" s="22"/>
     </row>
     <row r="40" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A40" s="5"/>
@@ -2011,16 +2034,16 @@
       <c r="C40" s="5"/>
       <c r="D40" s="5"/>
       <c r="E40" s="6"/>
-      <c r="F40" s="10"/>
-      <c r="G40" s="23"/>
+      <c r="F40" s="9"/>
+      <c r="G40" s="22"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" s="7"/>
       <c r="B41" s="7"/>
       <c r="C41" s="7"/>
       <c r="D41" s="7"/>
-      <c r="E41" s="11"/>
-      <c r="F41" s="12"/>
+      <c r="E41" s="10"/>
+      <c r="F41" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2044,7 +2067,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8585372C-4E8A-46A5-ABCB-0EC8F6702AC9}">
   <dimension ref="A1:A8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:A8"/>
     </sheetView>
   </sheetViews>

</xml_diff>